<commit_message>
added version arg, added error handling, made messages more consistent
</commit_message>
<xml_diff>
--- a/resources/Characters.xlsx
+++ b/resources/Characters.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DI_Projects\AMS_MI\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DI_Projects\g\xlsx-conv\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
-    <sheet name="Characters2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Euro sign (valuta format)</t>
   </si>
@@ -58,79 +57,20 @@
     <t>high bit ascii</t>
   </si>
   <si>
-    <t>405-2015</t>
-  </si>
-  <si>
-    <t>BBQ charcoal, briquettes, single use</t>
-  </si>
-  <si>
-    <t>Netto SE</t>
-  </si>
-  <si>
-    <t>X:\Non &amp; Near Food\Projects 2015\BBQ\09. Contracts\Confirmations\Savings Confirmations\Savings Confirmation BBQ 2015 DSG + DSG Netto.xlsx</t>
-  </si>
-  <si>
-    <t>302-2015</t>
-  </si>
-  <si>
-    <t>Bags, Foils and Filters</t>
-  </si>
-  <si>
-    <t>Albert Heijn</t>
-  </si>
-  <si>
-    <t>X:\Non &amp; Near Food\Projects 2015\Bags, foils and filters\09. Contracts\Confirmations\SCS approved\</t>
-  </si>
-  <si>
-    <t>X:\Non &amp; Near Food\Projects 2015\Bags, foils and filters\09. Contracts\Confirmations\SCS approved\Savings Confirmation Sphere (Asia) - AH 01.04.16-31.03.17 2602k</t>
-  </si>
-  <si>
-    <t>Project ID</t>
-  </si>
-  <si>
-    <t>PROJECT NAME</t>
-  </si>
-  <si>
-    <t>BUSINESS UNIT</t>
-  </si>
-  <si>
-    <t>Date Submitted</t>
-  </si>
-  <si>
-    <t>Concluded PV(CY) (Euro)</t>
-  </si>
-  <si>
-    <t>SCS.SOURCE</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Who?</t>
-  </si>
-  <si>
-    <t>201-2015</t>
-  </si>
-  <si>
-    <t>Beverage - Juices and Ice tea</t>
-  </si>
-  <si>
-    <t>X:\Food &amp; Beverages\Dry Groceries\Projects 2015\Juices\08. Contracts\SCS approved\SC - AMS Ambient Juices - AH NL - Valensina 25.01.2016-31.03.2016 (438.5)</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>Comma separated list</t>
+  </si>
+  <si>
+    <t>a, b, c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00000_ ;_ * \-#,##0.00000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.000;&quot;€&quot;\ \-#,##0.000"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ hh:mm"/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -156,18 +96,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -184,7 +118,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -192,17 +126,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -218,9 +146,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +186,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -330,7 +258,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -480,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G3"/>
+  <dimension ref="B2:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +419,7 @@
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -510,8 +438,11 @@
       <c r="G2" t="s">
         <v>9</v>
       </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1.123456789</v>
       </c>
@@ -526,6 +457,9 @@
       </c>
       <c r="G3" t="s">
         <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -535,135 +469,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="150.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="5">
-        <v>42205.407916666663</v>
-      </c>
-      <c r="E2" s="6">
-        <v>24000</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="5">
-        <v>42048.608611111114</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5">
-        <v>42339.422303240739</v>
-      </c>
-      <c r="E4" s="6">
-        <v>2602400</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="5">
-        <v>42389.394791666666</v>
-      </c>
-      <c r="E5" s="10">
-        <v>438500</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added option to replace linebreaks, ready for tagging 1.0.0
</commit_message>
<xml_diff>
--- a/resources/Characters.xlsx
+++ b/resources/Characters.xlsx
@@ -48,9 +48,6 @@
     <t>ends in backslash</t>
   </si>
   <si>
-    <t>C:\temp\</t>
-  </si>
-  <si>
     <t>ï of â</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>a, b, c</t>
+  </si>
+  <si>
+    <t>C:\temp\a,b\</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="B2:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,10 +436,10 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -453,13 +453,13 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added support for quoting output
</commit_message>
<xml_diff>
--- a/resources/Characters.xlsx
+++ b/resources/Characters.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DI_Projects\g\xlsx-conv\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Euro sign (valuta format)</t>
   </si>
@@ -61,21 +61,48 @@
   </si>
   <si>
     <t>C:\temp\a,b\</t>
+  </si>
+  <si>
+    <t>a "string" containing quotes</t>
+  </si>
+  <si>
+    <t>String with quotes</t>
+  </si>
+  <si>
+    <t>Semicolon in quotes</t>
+  </si>
+  <si>
+    <t>easy as "1;2;3"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00000_ ;_ * \-#,##0.00000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.000;&quot;€&quot;\ \-#,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,19 +145,20 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -407,64 +435,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1.123456789</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
#9 option to replace tab with replacement string
</commit_message>
<xml_diff>
--- a/resources/Characters.xlsx
+++ b/resources/Characters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DI_Projects\g\xlsx-conv\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Python\python-xlsx-conv\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1C5758-C72D-4AD5-9D3C-80527AB33E98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Euro sign (valuta format)</t>
   </si>
@@ -73,6 +74,9 @@
   </si>
   <si>
     <t>easy as "1;2;3"</t>
+  </si>
+  <si>
+    <t>Value with	tab</t>
   </si>
 </sst>
 </file>
@@ -145,7 +149,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -154,6 +158,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -439,17 +444,17 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +483,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1.123456789</v>
       </c>
@@ -487,6 +492,9 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>

</xml_diff>